<commit_message>
payment plan refactor (#4597)
</commit_message>
<xml_diff>
--- a/tests/unit/apps/registration_datahub/test_file/rdi_people_test.xlsx
+++ b/tests/unit/apps/registration_datahub/test_file/rdi_people_test.xlsx
@@ -1081,13 +1081,13 @@
     <t>pp_payment_delivery_phone_no_i_c</t>
   </si>
   <si>
-    <t>pp_card_number__atm_card_i_c</t>
-  </si>
-  <si>
-    <t>pp_card_expiry_date__atm_card_i_c</t>
-  </si>
-  <si>
-    <t>pp_name_of_cardholder__atm_card_i_c</t>
+    <t>pp_account__bank__card_number_i_c</t>
+  </si>
+  <si>
+    <t>pp_account__bank__card_expiry_date_i_c</t>
+  </si>
+  <si>
+    <t>pp_account__bank__name_of_cardholder_i_c</t>
   </si>
   <si>
     <t>pdu_string_attribute_round_1_value</t>
@@ -7303,13 +7303,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -7407,10 +7401,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -7656,13 +7650,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -7964,10 +7952,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -9235,7 +9223,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="70" width="8.85156" style="22" customWidth="1"/>
+    <col min="1" max="66" width="8.85156" style="22" customWidth="1"/>
+    <col min="67" max="67" width="34.7578" style="22" customWidth="1"/>
+    <col min="68" max="68" width="44.7109" style="22" customWidth="1"/>
+    <col min="69" max="69" width="35.7109" style="22" customWidth="1"/>
+    <col min="70" max="70" width="39.4375" style="22" customWidth="1"/>
     <col min="71" max="16384" width="8.85156" style="22" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>